<commit_message>
se completa la tabla para todos los reaseguradores
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/riesgo_credito.xlsx
+++ b/prototipo_pcr/inputs/riesgo_credito.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{9664797C-C4ED-204A-A0EC-16287C116FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E80440-EF77-5043-AED7-EB229F370CFC}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{9664797C-C4ED-204A-A0EC-16287C116FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7359A1A9-3611-1049-A3C2-C4912A62B966}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="3320" windowWidth="26040" windowHeight="14620" xr2:uid="{53D62D58-464B-AE40-ADC2-437A6FAD2003}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>fecha_inicio_vigencia</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>nit_reasegurador</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Ext</t>
+  </si>
+  <si>
+    <t>tipo_reasegurador</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8067C504-640E-054D-B661-D5C86A17E78E}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:I267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,7 +464,7 @@
     <col min="4" max="4" width="25.1640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45291</v>
       </c>
@@ -481,10 +490,10 @@
         <v>2374188</v>
       </c>
       <c r="D2" s="4">
-        <v>9.2799999999999994E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45322</v>
       </c>
@@ -496,10 +505,10 @@
         <v>2374188</v>
       </c>
       <c r="D3" s="4">
-        <v>8.8400000000000006E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45351</v>
       </c>
@@ -511,10 +520,10 @@
         <v>2374188</v>
       </c>
       <c r="D4" s="4">
-        <v>3.0700000000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45382</v>
       </c>
@@ -526,10 +535,10 @@
         <v>2374188</v>
       </c>
       <c r="D5" s="4">
-        <v>1.5699999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45412</v>
       </c>
@@ -541,10 +550,16 @@
         <v>2374188</v>
       </c>
       <c r="D6" s="4">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.04</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45443</v>
       </c>
@@ -556,10 +571,16 @@
         <v>2374188</v>
       </c>
       <c r="D7" s="4">
-        <v>3.5099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.06</v>
+      </c>
+      <c r="H7">
+        <v>2374188</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45473</v>
       </c>
@@ -571,10 +592,16 @@
         <v>2374188</v>
       </c>
       <c r="D8" s="4">
-        <v>1.4200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.03</v>
+      </c>
+      <c r="H8">
+        <v>6987458</v>
+      </c>
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45504</v>
       </c>
@@ -586,10 +613,16 @@
         <v>2374188</v>
       </c>
       <c r="D9" s="4">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.03</v>
+      </c>
+      <c r="H9">
+        <v>3693358</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45535</v>
       </c>
@@ -601,10 +634,16 @@
         <v>2374188</v>
       </c>
       <c r="D10" s="4">
-        <v>9.8400000000000001E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H10">
+        <v>3339928</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45565</v>
       </c>
@@ -616,10 +655,16 @@
         <v>2374188</v>
       </c>
       <c r="D11" s="4">
-        <v>8.3900000000000002E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.02</v>
+      </c>
+      <c r="H11">
+        <v>507351248</v>
+      </c>
+      <c r="I11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45596</v>
       </c>
@@ -631,10 +676,16 @@
         <v>2374188</v>
       </c>
       <c r="D12" s="4">
-        <v>2.4400000000000002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.02</v>
+      </c>
+      <c r="H12">
+        <v>368484453</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45626</v>
       </c>
@@ -646,10 +697,16 @@
         <v>2374188</v>
       </c>
       <c r="D13" s="4">
-        <v>4.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+      <c r="H13">
+        <v>446526767</v>
+      </c>
+      <c r="I13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45657</v>
       </c>
@@ -661,10 +718,16 @@
         <v>2374188</v>
       </c>
       <c r="D14" s="4">
-        <v>4.2200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.06</v>
+      </c>
+      <c r="H14">
+        <v>325775298</v>
+      </c>
+      <c r="I14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45688</v>
       </c>
@@ -676,10 +739,16 @@
         <v>2374188</v>
       </c>
       <c r="D15" s="4">
-        <v>9.5299999999999996E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.06</v>
+      </c>
+      <c r="H15">
+        <v>360681631</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45716</v>
       </c>
@@ -691,7 +760,7 @@
         <v>2374188</v>
       </c>
       <c r="D16" s="4">
-        <v>2.1499999999999998E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -706,7 +775,7 @@
         <v>2374188</v>
       </c>
       <c r="D17" s="4">
-        <v>9.11E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -721,7 +790,7 @@
         <v>2374188</v>
       </c>
       <c r="D18" s="4">
-        <v>9.6500000000000002E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -736,7 +805,7 @@
         <v>2374188</v>
       </c>
       <c r="D19" s="4">
-        <v>5.1700000000000003E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -751,7 +820,7 @@
         <v>2374188</v>
       </c>
       <c r="D20" s="4">
-        <v>6.3E-3</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -766,7 +835,7 @@
         <v>6987458</v>
       </c>
       <c r="D21" s="4">
-        <v>5.8200000000000002E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -781,7 +850,7 @@
         <v>6987458</v>
       </c>
       <c r="D22" s="4">
-        <v>2.0299999999999999E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -796,7 +865,7 @@
         <v>6987458</v>
       </c>
       <c r="D23" s="4">
-        <v>6.1999999999999998E-3</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -811,7 +880,7 @@
         <v>6987458</v>
       </c>
       <c r="D24" s="4">
-        <v>9.9900000000000003E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -826,7 +895,7 @@
         <v>6987458</v>
       </c>
       <c r="D25" s="4">
-        <v>3.1399999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,7 +910,7 @@
         <v>6987458</v>
       </c>
       <c r="D26" s="4">
-        <v>4.41E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -856,7 +925,7 @@
         <v>6987458</v>
       </c>
       <c r="D27" s="4">
-        <v>4.36E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -871,7 +940,7 @@
         <v>6987458</v>
       </c>
       <c r="D28" s="4">
-        <v>2.0899999999999998E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -886,7 +955,7 @@
         <v>6987458</v>
       </c>
       <c r="D29" s="4">
-        <v>2.9100000000000001E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -901,7 +970,7 @@
         <v>6987458</v>
       </c>
       <c r="D30" s="4">
-        <v>5.6899999999999999E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -916,7 +985,7 @@
         <v>6987458</v>
       </c>
       <c r="D31" s="4">
-        <v>2.75E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -931,7 +1000,7 @@
         <v>6987458</v>
       </c>
       <c r="D32" s="4">
-        <v>9.5600000000000004E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -946,7 +1015,7 @@
         <v>6987458</v>
       </c>
       <c r="D33" s="4">
-        <v>6.7699999999999996E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -961,7 +1030,7 @@
         <v>6987458</v>
       </c>
       <c r="D34" s="4">
-        <v>5.4100000000000002E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -976,7 +1045,7 @@
         <v>6987458</v>
       </c>
       <c r="D35" s="4">
-        <v>5.2600000000000001E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -991,7 +1060,7 @@
         <v>6987458</v>
       </c>
       <c r="D36" s="4">
-        <v>4.6399999999999997E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1006,7 +1075,7 @@
         <v>6987458</v>
       </c>
       <c r="D37" s="4">
-        <v>5.3199999999999997E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1021,7 +1090,7 @@
         <v>6987458</v>
       </c>
       <c r="D38" s="4">
-        <v>1.6500000000000001E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1036,7 +1105,7 @@
         <v>6987458</v>
       </c>
       <c r="D39" s="4">
-        <v>6.4100000000000004E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1051,7 +1120,7 @@
         <v>3693358</v>
       </c>
       <c r="D40" s="4">
-        <v>2.0000000000000001E-4</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1066,7 +1135,7 @@
         <v>3693358</v>
       </c>
       <c r="D41" s="4">
-        <v>9.1399999999999995E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1081,7 +1150,7 @@
         <v>3693358</v>
       </c>
       <c r="D42" s="4">
-        <v>8.8999999999999996E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1096,7 +1165,7 @@
         <v>3693358</v>
       </c>
       <c r="D43" s="4">
-        <v>2.64E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1111,7 +1180,7 @@
         <v>3693358</v>
       </c>
       <c r="D44" s="4">
-        <v>9.9000000000000005E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1126,7 +1195,7 @@
         <v>3693358</v>
       </c>
       <c r="D45" s="4">
-        <v>1.4E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1141,7 +1210,7 @@
         <v>3693358</v>
       </c>
       <c r="D46" s="4">
-        <v>9.0899999999999995E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1156,7 +1225,7 @@
         <v>3693358</v>
       </c>
       <c r="D47" s="4">
-        <v>4.1099999999999998E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1171,7 +1240,7 @@
         <v>3693358</v>
       </c>
       <c r="D48" s="4">
-        <v>6.8500000000000005E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1186,7 +1255,7 @@
         <v>3693358</v>
       </c>
       <c r="D49" s="4">
-        <v>8.4900000000000003E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1201,7 +1270,7 @@
         <v>3693358</v>
       </c>
       <c r="D50" s="4">
-        <v>1.2200000000000001E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1216,7 +1285,7 @@
         <v>3693358</v>
       </c>
       <c r="D51" s="4">
-        <v>4.19E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1231,7 +1300,7 @@
         <v>3693358</v>
       </c>
       <c r="D52" s="4">
-        <v>2.92E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1246,7 +1315,7 @@
         <v>3693358</v>
       </c>
       <c r="D53" s="4">
-        <v>6.9199999999999998E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1261,7 +1330,7 @@
         <v>3693358</v>
       </c>
       <c r="D54" s="4">
-        <v>9.7699999999999995E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1276,7 +1345,7 @@
         <v>3339928</v>
       </c>
       <c r="D55" s="4">
-        <v>8.9099999999999999E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1291,7 +1360,7 @@
         <v>3339928</v>
       </c>
       <c r="D56" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1306,7 +1375,7 @@
         <v>3339928</v>
       </c>
       <c r="D57" s="4">
-        <v>6.08E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1321,7 +1390,7 @@
         <v>3339928</v>
       </c>
       <c r="D58" s="4">
-        <v>5.7000000000000002E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1333,10 +1402,10 @@
         <v>45321</v>
       </c>
       <c r="C59">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D59" s="4">
-        <v>9.7000000000000003E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1348,10 +1417,10 @@
         <v>45350</v>
       </c>
       <c r="C60">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D60" s="4">
-        <v>9.1700000000000004E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1363,10 +1432,10 @@
         <v>45379</v>
       </c>
       <c r="C61">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D61" s="4">
-        <v>2.6499999999999999E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,10 +1447,10 @@
         <v>45411</v>
       </c>
       <c r="C62">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D62" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1393,10 +1462,10 @@
         <v>45441</v>
       </c>
       <c r="C63">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D63" s="4">
-        <v>2.9600000000000001E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1408,10 +1477,10 @@
         <v>45472</v>
       </c>
       <c r="C64">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D64" s="4">
-        <v>5.3199999999999997E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1423,10 +1492,10 @@
         <v>45502</v>
       </c>
       <c r="C65">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D65" s="4">
-        <v>7.3300000000000004E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1438,10 +1507,10 @@
         <v>45534</v>
       </c>
       <c r="C66">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D66" s="4">
-        <v>3.2500000000000001E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1453,10 +1522,10 @@
         <v>45564</v>
       </c>
       <c r="C67">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D67" s="4">
-        <v>5.8799999999999998E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1468,10 +1537,10 @@
         <v>45594</v>
       </c>
       <c r="C68">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D68" s="4">
-        <v>9.7100000000000006E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1483,10 +1552,10 @@
         <v>45625</v>
       </c>
       <c r="C69">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D69" s="4">
-        <v>2.06E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1498,10 +1567,10 @@
         <v>45655</v>
       </c>
       <c r="C70">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D70" s="4">
-        <v>4.5999999999999999E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1513,10 +1582,10 @@
         <v>45687</v>
       </c>
       <c r="C71">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D71" s="4">
-        <v>1.6799999999999999E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1528,10 +1597,10 @@
         <v>45715</v>
       </c>
       <c r="C72">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D72" s="4">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1543,10 +1612,10 @@
         <v>45743</v>
       </c>
       <c r="C73">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D73" s="4">
-        <v>3.2099999999999997E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1558,10 +1627,10 @@
         <v>45776</v>
       </c>
       <c r="C74">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D74" s="4">
-        <v>9.3799999999999994E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1573,10 +1642,10 @@
         <v>45806</v>
       </c>
       <c r="C75">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D75" s="4">
-        <v>5.6800000000000003E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1588,10 +1657,10 @@
         <v>45837</v>
       </c>
       <c r="C76">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D76" s="4">
-        <v>2.0199999999999999E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1603,10 +1672,2860 @@
         <v>45867</v>
       </c>
       <c r="C77">
-        <v>2374188</v>
+        <v>3693358</v>
       </c>
       <c r="D77" s="4">
-        <v>3.39E-2</v>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B78" s="2">
+        <f>+EDATE(A78,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C78">
+        <v>507351248</v>
+      </c>
+      <c r="D78" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B79" s="2">
+        <f t="shared" ref="B79:B115" si="2">+EDATE(A79,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C79">
+        <v>507351248</v>
+      </c>
+      <c r="D79" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B80" s="2">
+        <f t="shared" si="2"/>
+        <v>45379</v>
+      </c>
+      <c r="C80">
+        <v>507351248</v>
+      </c>
+      <c r="D80" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B81" s="2">
+        <f t="shared" si="2"/>
+        <v>45411</v>
+      </c>
+      <c r="C81">
+        <v>507351248</v>
+      </c>
+      <c r="D81" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B82" s="2">
+        <f t="shared" si="2"/>
+        <v>45441</v>
+      </c>
+      <c r="C82">
+        <v>507351248</v>
+      </c>
+      <c r="D82" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B83" s="2">
+        <f t="shared" si="2"/>
+        <v>45472</v>
+      </c>
+      <c r="C83">
+        <v>507351248</v>
+      </c>
+      <c r="D83" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B84" s="2">
+        <f t="shared" si="2"/>
+        <v>45502</v>
+      </c>
+      <c r="C84">
+        <v>507351248</v>
+      </c>
+      <c r="D84" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B85" s="2">
+        <f t="shared" si="2"/>
+        <v>45534</v>
+      </c>
+      <c r="C85">
+        <v>507351248</v>
+      </c>
+      <c r="D85" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B86" s="2">
+        <f t="shared" si="2"/>
+        <v>45564</v>
+      </c>
+      <c r="C86">
+        <v>507351248</v>
+      </c>
+      <c r="D86" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B87" s="2">
+        <f t="shared" si="2"/>
+        <v>45594</v>
+      </c>
+      <c r="C87">
+        <v>507351248</v>
+      </c>
+      <c r="D87" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B88" s="2">
+        <f t="shared" si="2"/>
+        <v>45625</v>
+      </c>
+      <c r="C88">
+        <v>507351248</v>
+      </c>
+      <c r="D88" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B89" s="2">
+        <f t="shared" si="2"/>
+        <v>45655</v>
+      </c>
+      <c r="C89">
+        <v>507351248</v>
+      </c>
+      <c r="D89" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B90" s="2">
+        <f t="shared" si="2"/>
+        <v>45687</v>
+      </c>
+      <c r="C90">
+        <v>507351248</v>
+      </c>
+      <c r="D90" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B91" s="2">
+        <f t="shared" si="2"/>
+        <v>45715</v>
+      </c>
+      <c r="C91">
+        <v>507351248</v>
+      </c>
+      <c r="D91" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B92" s="2">
+        <f t="shared" si="2"/>
+        <v>45743</v>
+      </c>
+      <c r="C92">
+        <v>507351248</v>
+      </c>
+      <c r="D92" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B93" s="2">
+        <f t="shared" si="2"/>
+        <v>45776</v>
+      </c>
+      <c r="C93">
+        <v>507351248</v>
+      </c>
+      <c r="D93" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B94" s="2">
+        <f t="shared" si="2"/>
+        <v>45806</v>
+      </c>
+      <c r="C94">
+        <v>507351248</v>
+      </c>
+      <c r="D94" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B95" s="2">
+        <f t="shared" si="2"/>
+        <v>45837</v>
+      </c>
+      <c r="C95">
+        <v>507351248</v>
+      </c>
+      <c r="D95" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B96" s="2">
+        <f t="shared" si="2"/>
+        <v>45867</v>
+      </c>
+      <c r="C96">
+        <v>507351248</v>
+      </c>
+      <c r="D96" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B97" s="2">
+        <f>+EDATE(A97,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C97">
+        <v>507351248</v>
+      </c>
+      <c r="D97" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B98" s="2">
+        <f t="shared" ref="B98:B115" si="3">+EDATE(A98,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C98">
+        <v>507351248</v>
+      </c>
+      <c r="D98" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B99" s="2">
+        <f t="shared" si="3"/>
+        <v>45379</v>
+      </c>
+      <c r="C99">
+        <v>507351248</v>
+      </c>
+      <c r="D99" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B100" s="2">
+        <f t="shared" si="3"/>
+        <v>45411</v>
+      </c>
+      <c r="C100">
+        <v>507351248</v>
+      </c>
+      <c r="D100" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B101" s="2">
+        <f t="shared" si="3"/>
+        <v>45441</v>
+      </c>
+      <c r="C101">
+        <v>507351248</v>
+      </c>
+      <c r="D101" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B102" s="2">
+        <f t="shared" si="3"/>
+        <v>45472</v>
+      </c>
+      <c r="C102">
+        <v>507351248</v>
+      </c>
+      <c r="D102" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B103" s="2">
+        <f t="shared" si="3"/>
+        <v>45502</v>
+      </c>
+      <c r="C103">
+        <v>507351248</v>
+      </c>
+      <c r="D103" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B104" s="2">
+        <f t="shared" si="3"/>
+        <v>45534</v>
+      </c>
+      <c r="C104">
+        <v>507351248</v>
+      </c>
+      <c r="D104" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B105" s="2">
+        <f t="shared" si="3"/>
+        <v>45564</v>
+      </c>
+      <c r="C105">
+        <v>507351248</v>
+      </c>
+      <c r="D105" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B106" s="2">
+        <f t="shared" si="3"/>
+        <v>45594</v>
+      </c>
+      <c r="C106">
+        <v>507351248</v>
+      </c>
+      <c r="D106" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B107" s="2">
+        <f t="shared" si="3"/>
+        <v>45625</v>
+      </c>
+      <c r="C107">
+        <v>507351248</v>
+      </c>
+      <c r="D107" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B108" s="2">
+        <f t="shared" si="3"/>
+        <v>45655</v>
+      </c>
+      <c r="C108">
+        <v>507351248</v>
+      </c>
+      <c r="D108" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B109" s="2">
+        <f t="shared" si="3"/>
+        <v>45687</v>
+      </c>
+      <c r="C109">
+        <v>507351248</v>
+      </c>
+      <c r="D109" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B110" s="2">
+        <f t="shared" si="3"/>
+        <v>45715</v>
+      </c>
+      <c r="C110">
+        <v>507351248</v>
+      </c>
+      <c r="D110" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B111" s="2">
+        <f t="shared" si="3"/>
+        <v>45743</v>
+      </c>
+      <c r="C111">
+        <v>507351248</v>
+      </c>
+      <c r="D111" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B112" s="2">
+        <f t="shared" si="3"/>
+        <v>45776</v>
+      </c>
+      <c r="C112">
+        <v>507351248</v>
+      </c>
+      <c r="D112" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B113" s="2">
+        <f t="shared" si="3"/>
+        <v>45806</v>
+      </c>
+      <c r="C113">
+        <v>507351248</v>
+      </c>
+      <c r="D113" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B114" s="2">
+        <f t="shared" si="3"/>
+        <v>45837</v>
+      </c>
+      <c r="C114">
+        <v>507351248</v>
+      </c>
+      <c r="D114" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B115" s="2">
+        <f t="shared" si="3"/>
+        <v>45867</v>
+      </c>
+      <c r="C115">
+        <v>507351248</v>
+      </c>
+      <c r="D115" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B116" s="2">
+        <f>+EDATE(A116,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C116">
+        <v>368484453</v>
+      </c>
+      <c r="D116" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B117" s="2">
+        <f t="shared" ref="B117:B153" si="4">+EDATE(A117,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C117">
+        <v>368484453</v>
+      </c>
+      <c r="D117" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B118" s="2">
+        <f t="shared" si="4"/>
+        <v>45379</v>
+      </c>
+      <c r="C118">
+        <v>368484453</v>
+      </c>
+      <c r="D118" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B119" s="2">
+        <f t="shared" si="4"/>
+        <v>45411</v>
+      </c>
+      <c r="C119">
+        <v>368484453</v>
+      </c>
+      <c r="D119" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B120" s="2">
+        <f t="shared" si="4"/>
+        <v>45441</v>
+      </c>
+      <c r="C120">
+        <v>368484453</v>
+      </c>
+      <c r="D120" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B121" s="2">
+        <f t="shared" si="4"/>
+        <v>45472</v>
+      </c>
+      <c r="C121">
+        <v>368484453</v>
+      </c>
+      <c r="D121" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B122" s="2">
+        <f t="shared" si="4"/>
+        <v>45502</v>
+      </c>
+      <c r="C122">
+        <v>368484453</v>
+      </c>
+      <c r="D122" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B123" s="2">
+        <f t="shared" si="4"/>
+        <v>45534</v>
+      </c>
+      <c r="C123">
+        <v>368484453</v>
+      </c>
+      <c r="D123" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B124" s="2">
+        <f t="shared" si="4"/>
+        <v>45564</v>
+      </c>
+      <c r="C124">
+        <v>368484453</v>
+      </c>
+      <c r="D124" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B125" s="2">
+        <f t="shared" si="4"/>
+        <v>45594</v>
+      </c>
+      <c r="C125">
+        <v>368484453</v>
+      </c>
+      <c r="D125" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B126" s="2">
+        <f t="shared" si="4"/>
+        <v>45625</v>
+      </c>
+      <c r="C126">
+        <v>368484453</v>
+      </c>
+      <c r="D126" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B127" s="2">
+        <f t="shared" si="4"/>
+        <v>45655</v>
+      </c>
+      <c r="C127">
+        <v>368484453</v>
+      </c>
+      <c r="D127" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B128" s="2">
+        <f t="shared" si="4"/>
+        <v>45687</v>
+      </c>
+      <c r="C128">
+        <v>368484453</v>
+      </c>
+      <c r="D128" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B129" s="2">
+        <f t="shared" si="4"/>
+        <v>45715</v>
+      </c>
+      <c r="C129">
+        <v>368484453</v>
+      </c>
+      <c r="D129" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B130" s="2">
+        <f t="shared" si="4"/>
+        <v>45743</v>
+      </c>
+      <c r="C130">
+        <v>368484453</v>
+      </c>
+      <c r="D130" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B131" s="2">
+        <f t="shared" si="4"/>
+        <v>45776</v>
+      </c>
+      <c r="C131">
+        <v>368484453</v>
+      </c>
+      <c r="D131" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B132" s="2">
+        <f t="shared" si="4"/>
+        <v>45806</v>
+      </c>
+      <c r="C132">
+        <v>368484453</v>
+      </c>
+      <c r="D132" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B133" s="2">
+        <f t="shared" si="4"/>
+        <v>45837</v>
+      </c>
+      <c r="C133">
+        <v>368484453</v>
+      </c>
+      <c r="D133" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B134" s="2">
+        <f t="shared" si="4"/>
+        <v>45867</v>
+      </c>
+      <c r="C134">
+        <v>368484453</v>
+      </c>
+      <c r="D134" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B135" s="2">
+        <f>+EDATE(A135,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C135">
+        <v>368484453</v>
+      </c>
+      <c r="D135" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B136" s="2">
+        <f t="shared" ref="B136:B153" si="5">+EDATE(A136,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C136">
+        <v>368484453</v>
+      </c>
+      <c r="D136" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B137" s="2">
+        <f t="shared" si="5"/>
+        <v>45379</v>
+      </c>
+      <c r="C137">
+        <v>368484453</v>
+      </c>
+      <c r="D137" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B138" s="2">
+        <f t="shared" si="5"/>
+        <v>45411</v>
+      </c>
+      <c r="C138">
+        <v>368484453</v>
+      </c>
+      <c r="D138" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B139" s="2">
+        <f t="shared" si="5"/>
+        <v>45441</v>
+      </c>
+      <c r="C139">
+        <v>368484453</v>
+      </c>
+      <c r="D139" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B140" s="2">
+        <f t="shared" si="5"/>
+        <v>45472</v>
+      </c>
+      <c r="C140">
+        <v>368484453</v>
+      </c>
+      <c r="D140" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B141" s="2">
+        <f t="shared" si="5"/>
+        <v>45502</v>
+      </c>
+      <c r="C141">
+        <v>368484453</v>
+      </c>
+      <c r="D141" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B142" s="2">
+        <f t="shared" si="5"/>
+        <v>45534</v>
+      </c>
+      <c r="C142">
+        <v>368484453</v>
+      </c>
+      <c r="D142" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B143" s="2">
+        <f t="shared" si="5"/>
+        <v>45564</v>
+      </c>
+      <c r="C143">
+        <v>368484453</v>
+      </c>
+      <c r="D143" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B144" s="2">
+        <f t="shared" si="5"/>
+        <v>45594</v>
+      </c>
+      <c r="C144">
+        <v>368484453</v>
+      </c>
+      <c r="D144" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B145" s="2">
+        <f t="shared" si="5"/>
+        <v>45625</v>
+      </c>
+      <c r="C145">
+        <v>368484453</v>
+      </c>
+      <c r="D145" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B146" s="2">
+        <f t="shared" si="5"/>
+        <v>45655</v>
+      </c>
+      <c r="C146">
+        <v>368484453</v>
+      </c>
+      <c r="D146" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B147" s="2">
+        <f t="shared" si="5"/>
+        <v>45687</v>
+      </c>
+      <c r="C147">
+        <v>368484453</v>
+      </c>
+      <c r="D147" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B148" s="2">
+        <f t="shared" si="5"/>
+        <v>45715</v>
+      </c>
+      <c r="C148">
+        <v>368484453</v>
+      </c>
+      <c r="D148" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B149" s="2">
+        <f t="shared" si="5"/>
+        <v>45743</v>
+      </c>
+      <c r="C149">
+        <v>368484453</v>
+      </c>
+      <c r="D149" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B150" s="2">
+        <f t="shared" si="5"/>
+        <v>45776</v>
+      </c>
+      <c r="C150">
+        <v>368484453</v>
+      </c>
+      <c r="D150" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B151" s="2">
+        <f t="shared" si="5"/>
+        <v>45806</v>
+      </c>
+      <c r="C151">
+        <v>368484453</v>
+      </c>
+      <c r="D151" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B152" s="2">
+        <f t="shared" si="5"/>
+        <v>45837</v>
+      </c>
+      <c r="C152">
+        <v>368484453</v>
+      </c>
+      <c r="D152" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B153" s="2">
+        <f t="shared" si="5"/>
+        <v>45867</v>
+      </c>
+      <c r="C153">
+        <v>368484453</v>
+      </c>
+      <c r="D153" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B154" s="2">
+        <f>+EDATE(A154,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C154">
+        <v>446526767</v>
+      </c>
+      <c r="D154" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B155" s="2">
+        <f t="shared" ref="B155:B191" si="6">+EDATE(A155,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C155">
+        <v>446526767</v>
+      </c>
+      <c r="D155" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B156" s="2">
+        <f t="shared" si="6"/>
+        <v>45379</v>
+      </c>
+      <c r="C156">
+        <v>446526767</v>
+      </c>
+      <c r="D156" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B157" s="2">
+        <f t="shared" si="6"/>
+        <v>45411</v>
+      </c>
+      <c r="C157">
+        <v>446526767</v>
+      </c>
+      <c r="D157" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B158" s="2">
+        <f t="shared" si="6"/>
+        <v>45441</v>
+      </c>
+      <c r="C158">
+        <v>446526767</v>
+      </c>
+      <c r="D158" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B159" s="2">
+        <f t="shared" si="6"/>
+        <v>45472</v>
+      </c>
+      <c r="C159">
+        <v>446526767</v>
+      </c>
+      <c r="D159" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B160" s="2">
+        <f t="shared" si="6"/>
+        <v>45502</v>
+      </c>
+      <c r="C160">
+        <v>446526767</v>
+      </c>
+      <c r="D160" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B161" s="2">
+        <f t="shared" si="6"/>
+        <v>45534</v>
+      </c>
+      <c r="C161">
+        <v>446526767</v>
+      </c>
+      <c r="D161" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B162" s="2">
+        <f t="shared" si="6"/>
+        <v>45564</v>
+      </c>
+      <c r="C162">
+        <v>446526767</v>
+      </c>
+      <c r="D162" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B163" s="2">
+        <f t="shared" si="6"/>
+        <v>45594</v>
+      </c>
+      <c r="C163">
+        <v>446526767</v>
+      </c>
+      <c r="D163" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B164" s="2">
+        <f t="shared" si="6"/>
+        <v>45625</v>
+      </c>
+      <c r="C164">
+        <v>446526767</v>
+      </c>
+      <c r="D164" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B165" s="2">
+        <f t="shared" si="6"/>
+        <v>45655</v>
+      </c>
+      <c r="C165">
+        <v>446526767</v>
+      </c>
+      <c r="D165" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B166" s="2">
+        <f t="shared" si="6"/>
+        <v>45687</v>
+      </c>
+      <c r="C166">
+        <v>446526767</v>
+      </c>
+      <c r="D166" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B167" s="2">
+        <f t="shared" si="6"/>
+        <v>45715</v>
+      </c>
+      <c r="C167">
+        <v>446526767</v>
+      </c>
+      <c r="D167" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B168" s="2">
+        <f t="shared" si="6"/>
+        <v>45743</v>
+      </c>
+      <c r="C168">
+        <v>446526767</v>
+      </c>
+      <c r="D168" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B169" s="2">
+        <f t="shared" si="6"/>
+        <v>45776</v>
+      </c>
+      <c r="C169">
+        <v>446526767</v>
+      </c>
+      <c r="D169" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B170" s="2">
+        <f t="shared" si="6"/>
+        <v>45806</v>
+      </c>
+      <c r="C170">
+        <v>446526767</v>
+      </c>
+      <c r="D170" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B171" s="2">
+        <f t="shared" si="6"/>
+        <v>45837</v>
+      </c>
+      <c r="C171">
+        <v>446526767</v>
+      </c>
+      <c r="D171" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B172" s="2">
+        <f t="shared" si="6"/>
+        <v>45867</v>
+      </c>
+      <c r="C172">
+        <v>446526767</v>
+      </c>
+      <c r="D172" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B173" s="2">
+        <f>+EDATE(A173,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C173">
+        <v>446526767</v>
+      </c>
+      <c r="D173" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B174" s="2">
+        <f t="shared" ref="B174:B191" si="7">+EDATE(A174,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C174">
+        <v>446526767</v>
+      </c>
+      <c r="D174" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B175" s="2">
+        <f t="shared" si="7"/>
+        <v>45379</v>
+      </c>
+      <c r="C175">
+        <v>446526767</v>
+      </c>
+      <c r="D175" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B176" s="2">
+        <f t="shared" si="7"/>
+        <v>45411</v>
+      </c>
+      <c r="C176">
+        <v>446526767</v>
+      </c>
+      <c r="D176" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B177" s="2">
+        <f t="shared" si="7"/>
+        <v>45441</v>
+      </c>
+      <c r="C177">
+        <v>446526767</v>
+      </c>
+      <c r="D177" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B178" s="2">
+        <f t="shared" si="7"/>
+        <v>45472</v>
+      </c>
+      <c r="C178">
+        <v>446526767</v>
+      </c>
+      <c r="D178" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B179" s="2">
+        <f t="shared" si="7"/>
+        <v>45502</v>
+      </c>
+      <c r="C179">
+        <v>446526767</v>
+      </c>
+      <c r="D179" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B180" s="2">
+        <f t="shared" si="7"/>
+        <v>45534</v>
+      </c>
+      <c r="C180">
+        <v>446526767</v>
+      </c>
+      <c r="D180" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B181" s="2">
+        <f t="shared" si="7"/>
+        <v>45564</v>
+      </c>
+      <c r="C181">
+        <v>446526767</v>
+      </c>
+      <c r="D181" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B182" s="2">
+        <f t="shared" si="7"/>
+        <v>45594</v>
+      </c>
+      <c r="C182">
+        <v>446526767</v>
+      </c>
+      <c r="D182" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B183" s="2">
+        <f t="shared" si="7"/>
+        <v>45625</v>
+      </c>
+      <c r="C183">
+        <v>446526767</v>
+      </c>
+      <c r="D183" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B184" s="2">
+        <f t="shared" si="7"/>
+        <v>45655</v>
+      </c>
+      <c r="C184">
+        <v>446526767</v>
+      </c>
+      <c r="D184" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B185" s="2">
+        <f t="shared" si="7"/>
+        <v>45687</v>
+      </c>
+      <c r="C185">
+        <v>446526767</v>
+      </c>
+      <c r="D185" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B186" s="2">
+        <f t="shared" si="7"/>
+        <v>45715</v>
+      </c>
+      <c r="C186">
+        <v>446526767</v>
+      </c>
+      <c r="D186" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B187" s="2">
+        <f t="shared" si="7"/>
+        <v>45743</v>
+      </c>
+      <c r="C187">
+        <v>446526767</v>
+      </c>
+      <c r="D187" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B188" s="2">
+        <f t="shared" si="7"/>
+        <v>45776</v>
+      </c>
+      <c r="C188">
+        <v>446526767</v>
+      </c>
+      <c r="D188" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B189" s="2">
+        <f t="shared" si="7"/>
+        <v>45806</v>
+      </c>
+      <c r="C189">
+        <v>446526767</v>
+      </c>
+      <c r="D189" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B190" s="2">
+        <f t="shared" si="7"/>
+        <v>45837</v>
+      </c>
+      <c r="C190">
+        <v>446526767</v>
+      </c>
+      <c r="D190" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B191" s="2">
+        <f t="shared" si="7"/>
+        <v>45867</v>
+      </c>
+      <c r="C191">
+        <v>446526767</v>
+      </c>
+      <c r="D191" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B192" s="2">
+        <f>+EDATE(A192,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C192">
+        <v>325775298</v>
+      </c>
+      <c r="D192" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B193" s="2">
+        <f t="shared" ref="B193:B229" si="8">+EDATE(A193,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C193">
+        <v>325775298</v>
+      </c>
+      <c r="D193" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B194" s="2">
+        <f t="shared" si="8"/>
+        <v>45379</v>
+      </c>
+      <c r="C194">
+        <v>325775298</v>
+      </c>
+      <c r="D194" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B195" s="2">
+        <f t="shared" si="8"/>
+        <v>45411</v>
+      </c>
+      <c r="C195">
+        <v>325775298</v>
+      </c>
+      <c r="D195" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B196" s="2">
+        <f t="shared" si="8"/>
+        <v>45441</v>
+      </c>
+      <c r="C196">
+        <v>325775298</v>
+      </c>
+      <c r="D196" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B197" s="2">
+        <f t="shared" si="8"/>
+        <v>45472</v>
+      </c>
+      <c r="C197">
+        <v>325775298</v>
+      </c>
+      <c r="D197" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B198" s="2">
+        <f t="shared" si="8"/>
+        <v>45502</v>
+      </c>
+      <c r="C198">
+        <v>325775298</v>
+      </c>
+      <c r="D198" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B199" s="2">
+        <f t="shared" si="8"/>
+        <v>45534</v>
+      </c>
+      <c r="C199">
+        <v>325775298</v>
+      </c>
+      <c r="D199" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B200" s="2">
+        <f t="shared" si="8"/>
+        <v>45564</v>
+      </c>
+      <c r="C200">
+        <v>325775298</v>
+      </c>
+      <c r="D200" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B201" s="2">
+        <f t="shared" si="8"/>
+        <v>45594</v>
+      </c>
+      <c r="C201">
+        <v>325775298</v>
+      </c>
+      <c r="D201" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B202" s="2">
+        <f t="shared" si="8"/>
+        <v>45625</v>
+      </c>
+      <c r="C202">
+        <v>325775298</v>
+      </c>
+      <c r="D202" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B203" s="2">
+        <f t="shared" si="8"/>
+        <v>45655</v>
+      </c>
+      <c r="C203">
+        <v>325775298</v>
+      </c>
+      <c r="D203" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B204" s="2">
+        <f t="shared" si="8"/>
+        <v>45687</v>
+      </c>
+      <c r="C204">
+        <v>325775298</v>
+      </c>
+      <c r="D204" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B205" s="2">
+        <f t="shared" si="8"/>
+        <v>45715</v>
+      </c>
+      <c r="C205">
+        <v>325775298</v>
+      </c>
+      <c r="D205" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B206" s="2">
+        <f t="shared" si="8"/>
+        <v>45743</v>
+      </c>
+      <c r="C206">
+        <v>325775298</v>
+      </c>
+      <c r="D206" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B207" s="2">
+        <f t="shared" si="8"/>
+        <v>45776</v>
+      </c>
+      <c r="C207">
+        <v>325775298</v>
+      </c>
+      <c r="D207" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B208" s="2">
+        <f t="shared" si="8"/>
+        <v>45806</v>
+      </c>
+      <c r="C208">
+        <v>325775298</v>
+      </c>
+      <c r="D208" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B209" s="2">
+        <f t="shared" si="8"/>
+        <v>45837</v>
+      </c>
+      <c r="C209">
+        <v>325775298</v>
+      </c>
+      <c r="D209" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B210" s="2">
+        <f t="shared" si="8"/>
+        <v>45867</v>
+      </c>
+      <c r="C210">
+        <v>325775298</v>
+      </c>
+      <c r="D210" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B211" s="2">
+        <f>+EDATE(A211,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C211">
+        <v>325775298</v>
+      </c>
+      <c r="D211" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B212" s="2">
+        <f t="shared" ref="B212:B229" si="9">+EDATE(A212,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C212">
+        <v>325775298</v>
+      </c>
+      <c r="D212" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B213" s="2">
+        <f t="shared" si="9"/>
+        <v>45379</v>
+      </c>
+      <c r="C213">
+        <v>325775298</v>
+      </c>
+      <c r="D213" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B214" s="2">
+        <f t="shared" si="9"/>
+        <v>45411</v>
+      </c>
+      <c r="C214">
+        <v>325775298</v>
+      </c>
+      <c r="D214" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B215" s="2">
+        <f t="shared" si="9"/>
+        <v>45441</v>
+      </c>
+      <c r="C215">
+        <v>325775298</v>
+      </c>
+      <c r="D215" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B216" s="2">
+        <f t="shared" si="9"/>
+        <v>45472</v>
+      </c>
+      <c r="C216">
+        <v>325775298</v>
+      </c>
+      <c r="D216" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B217" s="2">
+        <f t="shared" si="9"/>
+        <v>45502</v>
+      </c>
+      <c r="C217">
+        <v>325775298</v>
+      </c>
+      <c r="D217" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B218" s="2">
+        <f t="shared" si="9"/>
+        <v>45534</v>
+      </c>
+      <c r="C218">
+        <v>325775298</v>
+      </c>
+      <c r="D218" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B219" s="2">
+        <f t="shared" si="9"/>
+        <v>45564</v>
+      </c>
+      <c r="C219">
+        <v>325775298</v>
+      </c>
+      <c r="D219" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B220" s="2">
+        <f t="shared" si="9"/>
+        <v>45594</v>
+      </c>
+      <c r="C220">
+        <v>325775298</v>
+      </c>
+      <c r="D220" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B221" s="2">
+        <f t="shared" si="9"/>
+        <v>45625</v>
+      </c>
+      <c r="C221">
+        <v>325775298</v>
+      </c>
+      <c r="D221" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B222" s="2">
+        <f t="shared" si="9"/>
+        <v>45655</v>
+      </c>
+      <c r="C222">
+        <v>325775298</v>
+      </c>
+      <c r="D222" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B223" s="2">
+        <f t="shared" si="9"/>
+        <v>45687</v>
+      </c>
+      <c r="C223">
+        <v>325775298</v>
+      </c>
+      <c r="D223" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B224" s="2">
+        <f t="shared" si="9"/>
+        <v>45715</v>
+      </c>
+      <c r="C224">
+        <v>325775298</v>
+      </c>
+      <c r="D224" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B225" s="2">
+        <f t="shared" si="9"/>
+        <v>45743</v>
+      </c>
+      <c r="C225">
+        <v>325775298</v>
+      </c>
+      <c r="D225" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B226" s="2">
+        <f t="shared" si="9"/>
+        <v>45776</v>
+      </c>
+      <c r="C226">
+        <v>325775298</v>
+      </c>
+      <c r="D226" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B227" s="2">
+        <f t="shared" si="9"/>
+        <v>45806</v>
+      </c>
+      <c r="C227">
+        <v>325775298</v>
+      </c>
+      <c r="D227" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B228" s="2">
+        <f t="shared" si="9"/>
+        <v>45837</v>
+      </c>
+      <c r="C228">
+        <v>325775298</v>
+      </c>
+      <c r="D228" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B229" s="2">
+        <f t="shared" si="9"/>
+        <v>45867</v>
+      </c>
+      <c r="C229">
+        <v>325775298</v>
+      </c>
+      <c r="D229" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B230" s="2">
+        <f>+EDATE(A230,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C230">
+        <v>360681631</v>
+      </c>
+      <c r="D230" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B231" s="2">
+        <f t="shared" ref="B231:B267" si="10">+EDATE(A231,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C231">
+        <v>360681631</v>
+      </c>
+      <c r="D231" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B232" s="2">
+        <f t="shared" si="10"/>
+        <v>45379</v>
+      </c>
+      <c r="C232">
+        <v>360681631</v>
+      </c>
+      <c r="D232" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B233" s="2">
+        <f t="shared" si="10"/>
+        <v>45411</v>
+      </c>
+      <c r="C233">
+        <v>360681631</v>
+      </c>
+      <c r="D233" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B234" s="2">
+        <f t="shared" si="10"/>
+        <v>45441</v>
+      </c>
+      <c r="C234">
+        <v>360681631</v>
+      </c>
+      <c r="D234" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B235" s="2">
+        <f t="shared" si="10"/>
+        <v>45472</v>
+      </c>
+      <c r="C235">
+        <v>360681631</v>
+      </c>
+      <c r="D235" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B236" s="2">
+        <f t="shared" si="10"/>
+        <v>45502</v>
+      </c>
+      <c r="C236">
+        <v>360681631</v>
+      </c>
+      <c r="D236" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B237" s="2">
+        <f t="shared" si="10"/>
+        <v>45534</v>
+      </c>
+      <c r="C237">
+        <v>360681631</v>
+      </c>
+      <c r="D237" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B238" s="2">
+        <f t="shared" si="10"/>
+        <v>45564</v>
+      </c>
+      <c r="C238">
+        <v>360681631</v>
+      </c>
+      <c r="D238" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B239" s="2">
+        <f t="shared" si="10"/>
+        <v>45594</v>
+      </c>
+      <c r="C239">
+        <v>360681631</v>
+      </c>
+      <c r="D239" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B240" s="2">
+        <f t="shared" si="10"/>
+        <v>45625</v>
+      </c>
+      <c r="C240">
+        <v>360681631</v>
+      </c>
+      <c r="D240" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B241" s="2">
+        <f t="shared" si="10"/>
+        <v>45655</v>
+      </c>
+      <c r="C241">
+        <v>360681631</v>
+      </c>
+      <c r="D241" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B242" s="2">
+        <f t="shared" si="10"/>
+        <v>45687</v>
+      </c>
+      <c r="C242">
+        <v>360681631</v>
+      </c>
+      <c r="D242" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B243" s="2">
+        <f t="shared" si="10"/>
+        <v>45715</v>
+      </c>
+      <c r="C243">
+        <v>360681631</v>
+      </c>
+      <c r="D243" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B244" s="2">
+        <f t="shared" si="10"/>
+        <v>45743</v>
+      </c>
+      <c r="C244">
+        <v>360681631</v>
+      </c>
+      <c r="D244" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B245" s="2">
+        <f t="shared" si="10"/>
+        <v>45776</v>
+      </c>
+      <c r="C245">
+        <v>360681631</v>
+      </c>
+      <c r="D245" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B246" s="2">
+        <f t="shared" si="10"/>
+        <v>45806</v>
+      </c>
+      <c r="C246">
+        <v>360681631</v>
+      </c>
+      <c r="D246" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B247" s="2">
+        <f t="shared" si="10"/>
+        <v>45837</v>
+      </c>
+      <c r="C247">
+        <v>360681631</v>
+      </c>
+      <c r="D247" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B248" s="2">
+        <f t="shared" si="10"/>
+        <v>45867</v>
+      </c>
+      <c r="C248">
+        <v>360681631</v>
+      </c>
+      <c r="D248" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B249" s="2">
+        <f>+EDATE(A249,1)-1</f>
+        <v>45321</v>
+      </c>
+      <c r="C249">
+        <v>360681631</v>
+      </c>
+      <c r="D249" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B250" s="2">
+        <f t="shared" ref="B250:B267" si="11">+EDATE(A250,1)-1</f>
+        <v>45350</v>
+      </c>
+      <c r="C250">
+        <v>360681631</v>
+      </c>
+      <c r="D250" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B251" s="2">
+        <f t="shared" si="11"/>
+        <v>45379</v>
+      </c>
+      <c r="C251">
+        <v>360681631</v>
+      </c>
+      <c r="D251" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252" s="2">
+        <v>45382</v>
+      </c>
+      <c r="B252" s="2">
+        <f t="shared" si="11"/>
+        <v>45411</v>
+      </c>
+      <c r="C252">
+        <v>360681631</v>
+      </c>
+      <c r="D252" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B253" s="2">
+        <f t="shared" si="11"/>
+        <v>45441</v>
+      </c>
+      <c r="C253">
+        <v>360681631</v>
+      </c>
+      <c r="D253" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B254" s="2">
+        <f t="shared" si="11"/>
+        <v>45472</v>
+      </c>
+      <c r="C254">
+        <v>360681631</v>
+      </c>
+      <c r="D254" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" s="2">
+        <v>45473</v>
+      </c>
+      <c r="B255" s="2">
+        <f t="shared" si="11"/>
+        <v>45502</v>
+      </c>
+      <c r="C255">
+        <v>360681631</v>
+      </c>
+      <c r="D255" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="2">
+        <v>45504</v>
+      </c>
+      <c r="B256" s="2">
+        <f t="shared" si="11"/>
+        <v>45534</v>
+      </c>
+      <c r="C256">
+        <v>360681631</v>
+      </c>
+      <c r="D256" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B257" s="2">
+        <f t="shared" si="11"/>
+        <v>45564</v>
+      </c>
+      <c r="C257">
+        <v>360681631</v>
+      </c>
+      <c r="D257" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B258" s="2">
+        <f t="shared" si="11"/>
+        <v>45594</v>
+      </c>
+      <c r="C258">
+        <v>360681631</v>
+      </c>
+      <c r="D258" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B259" s="2">
+        <f t="shared" si="11"/>
+        <v>45625</v>
+      </c>
+      <c r="C259">
+        <v>360681631</v>
+      </c>
+      <c r="D259" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B260" s="2">
+        <f t="shared" si="11"/>
+        <v>45655</v>
+      </c>
+      <c r="C260">
+        <v>360681631</v>
+      </c>
+      <c r="D260" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B261" s="2">
+        <f t="shared" si="11"/>
+        <v>45687</v>
+      </c>
+      <c r="C261">
+        <v>360681631</v>
+      </c>
+      <c r="D261" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B262" s="2">
+        <f t="shared" si="11"/>
+        <v>45715</v>
+      </c>
+      <c r="C262">
+        <v>360681631</v>
+      </c>
+      <c r="D262" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B263" s="2">
+        <f t="shared" si="11"/>
+        <v>45743</v>
+      </c>
+      <c r="C263">
+        <v>360681631</v>
+      </c>
+      <c r="D263" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B264" s="2">
+        <f t="shared" si="11"/>
+        <v>45776</v>
+      </c>
+      <c r="C264">
+        <v>360681631</v>
+      </c>
+      <c r="D264" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" s="2">
+        <v>45777</v>
+      </c>
+      <c r="B265" s="2">
+        <f t="shared" si="11"/>
+        <v>45806</v>
+      </c>
+      <c r="C265">
+        <v>360681631</v>
+      </c>
+      <c r="D265" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="2">
+        <v>45808</v>
+      </c>
+      <c r="B266" s="2">
+        <f t="shared" si="11"/>
+        <v>45837</v>
+      </c>
+      <c r="C266">
+        <v>360681631</v>
+      </c>
+      <c r="D266" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B267" s="2">
+        <f t="shared" si="11"/>
+        <v>45867</v>
+      </c>
+      <c r="C267">
+        <v>360681631</v>
+      </c>
+      <c r="D267" s="4">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -1615,12 +4534,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1825,20 +4746,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6902C395-3E7F-46E5-962F-00112FC449C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B5B73F0-0F51-4D90-98B1-6FD6C9B96585}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1863,18 +4791,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B5B73F0-0F51-4D90-98B1-6FD6C9B96585}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6902C395-3E7F-46E5-962F-00112FC449C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
se ajusta insumo riesgo credito
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/riesgo_credito.xlsx
+++ b/prototipo_pcr/inputs/riesgo_credito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/TraNIFF/Shared Documents/féniX/01 IFRS17/02 Entregables Procesos/05 Reservas/03 PCR CP/03 Tecnología/01 Prototipo/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{9664797C-C4ED-204A-A0EC-16287C116FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7359A1A9-3611-1049-A3C2-C4912A62B966}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{9664797C-C4ED-204A-A0EC-16287C116FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFF079DF-5ADA-AD42-841E-C84CF68FB277}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="3320" windowWidth="26040" windowHeight="14620" xr2:uid="{53D62D58-464B-AE40-ADC2-437A6FAD2003}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>fecha_inicio_vigencia</t>
   </si>
@@ -48,15 +48,6 @@
   </si>
   <si>
     <t>nit_reasegurador</t>
-  </si>
-  <si>
-    <t>Int</t>
-  </si>
-  <si>
-    <t>Ext</t>
-  </si>
-  <si>
-    <t>tipo_reasegurador</t>
   </si>
 </sst>
 </file>
@@ -454,7 +445,7 @@
   <dimension ref="A1:I267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H6" sqref="H6:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,12 +543,8 @@
       <c r="D6" s="4">
         <v>0.04</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -573,12 +560,6 @@
       <c r="D7" s="4">
         <v>0.06</v>
       </c>
-      <c r="H7">
-        <v>2374188</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -594,12 +575,6 @@
       <c r="D8" s="4">
         <v>0.03</v>
       </c>
-      <c r="H8">
-        <v>6987458</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -615,12 +590,6 @@
       <c r="D9" s="4">
         <v>0.03</v>
       </c>
-      <c r="H9">
-        <v>3693358</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -636,12 +605,6 @@
       <c r="D10" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H10">
-        <v>3339928</v>
-      </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -657,12 +620,6 @@
       <c r="D11" s="4">
         <v>0.02</v>
       </c>
-      <c r="H11">
-        <v>507351248</v>
-      </c>
-      <c r="I11" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -678,12 +635,6 @@
       <c r="D12" s="4">
         <v>0.02</v>
       </c>
-      <c r="H12">
-        <v>368484453</v>
-      </c>
-      <c r="I12" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -699,12 +650,6 @@
       <c r="D13" s="4">
         <v>0.01</v>
       </c>
-      <c r="H13">
-        <v>446526767</v>
-      </c>
-      <c r="I13" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -720,12 +665,6 @@
       <c r="D14" s="4">
         <v>0.06</v>
       </c>
-      <c r="H14">
-        <v>325775298</v>
-      </c>
-      <c r="I14" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -740,12 +679,6 @@
       </c>
       <c r="D15" s="4">
         <v>0.06</v>
-      </c>
-      <c r="H15">
-        <v>360681631</v>
-      </c>
-      <c r="I15" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>